<commit_message>
Change a little for formal work (not done).
</commit_message>
<xml_diff>
--- a/pollen_tokyo-osaka.xlsx
+++ b/pollen_tokyo-osaka.xlsx
@@ -456,7 +456,7 @@
         <v>43107</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
@@ -467,10 +467,10 @@
         <v>43114</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         <v>43121</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -511,10 +511,10 @@
         <v>43142</v>
       </c>
       <c r="B7" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -522,10 +522,10 @@
         <v>43149</v>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -533,10 +533,10 @@
         <v>43156</v>
       </c>
       <c r="B9" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
@@ -544,10 +544,10 @@
         <v>43163</v>
       </c>
       <c r="B10" t="n">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C10" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         <v>43177</v>
       </c>
       <c r="B12" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
@@ -577,10 +577,10 @@
         <v>43184</v>
       </c>
       <c r="B13" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C13" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -588,10 +588,10 @@
         <v>43191</v>
       </c>
       <c r="B14" t="n">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
@@ -610,10 +610,10 @@
         <v>43205</v>
       </c>
       <c r="B16" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -621,10 +621,10 @@
         <v>43212</v>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -632,10 +632,10 @@
         <v>43219</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -643,10 +643,10 @@
         <v>43226</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -654,10 +654,10 @@
         <v>43233</v>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
@@ -665,7 +665,7 @@
         <v>43240</v>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
         <v>6</v>
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -731,7 +731,7 @@
         <v>43282</v>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
@@ -742,10 +742,10 @@
         <v>43289</v>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -753,10 +753,10 @@
         <v>43296</v>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -786,10 +786,10 @@
         <v>43317</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -830,10 +830,10 @@
         <v>43345</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -852,7 +852,7 @@
         <v>43359</v>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" t="n">
         <v>3</v>
@@ -863,10 +863,10 @@
         <v>43366</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -874,10 +874,10 @@
         <v>43373</v>
       </c>
       <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="n">
         <v>4</v>
-      </c>
-      <c r="C40" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -899,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
@@ -918,10 +918,10 @@
         <v>43401</v>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -932,7 +932,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -943,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -973,7 +973,7 @@
         <v>43436</v>
       </c>
       <c r="B49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
         <v>2</v>
@@ -984,10 +984,10 @@
         <v>43443</v>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -998,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1006,10 +1006,10 @@
         <v>43457</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1017,10 +1017,10 @@
         <v>43464</v>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>